<commit_message>
BOM with 2017 re-order
</commit_message>
<xml_diff>
--- a/elec/bom/BlueBoard_v1_bom.xlsx
+++ b/elec/bom/BlueBoard_v1_bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="241">
   <si>
     <t>Value</t>
   </si>
@@ -606,9 +606,6 @@
     <t>R28, R32, R64, R65, R66, R67, R78</t>
   </si>
   <si>
-    <t>LED4, LED5, LED6, LED7, LED8, LED9</t>
-  </si>
-  <si>
     <t>Parts</t>
   </si>
   <si>
@@ -685,6 +682,63 @@
   </si>
   <si>
     <t>510k</t>
+  </si>
+  <si>
+    <t>Achats 2017</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>LED4, LED5, LED6</t>
+  </si>
+  <si>
+    <t>LED7, LED8, LED9</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>Panier</t>
+  </si>
+  <si>
+    <t>Nb</t>
+  </si>
+  <si>
+    <t>HMHA2801R2</t>
+  </si>
+  <si>
+    <t>SAMPLE TODO</t>
+  </si>
+  <si>
+    <t>MODULE PRINCE</t>
+  </si>
+  <si>
+    <t>appro x2</t>
+  </si>
+  <si>
+    <t>correspondance: 1792847</t>
+  </si>
+  <si>
+    <t>correspondance: 1792849</t>
+  </si>
+  <si>
+    <t>changement 1716766</t>
+  </si>
+  <si>
+    <t>remplacé</t>
+  </si>
+  <si>
+    <t>remplacé par 10 uF</t>
   </si>
 </sst>
 </file>
@@ -765,7 +819,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,11 +838,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -798,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -830,6 +929,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -916,8 +1027,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I64" totalsRowShown="0">
-  <autoFilter ref="A4:I64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I65" totalsRowShown="0">
+  <autoFilter ref="A4:I65">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
     <filterColumn colId="8"/>
@@ -1227,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L224"/>
+  <dimension ref="A1:R225"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <selection pane="bottomLeft" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1245,14 +1356,17 @@
     <col min="7" max="7" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="11" max="12" width="3.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21">
+    <row r="1" spans="1:18" ht="21">
       <c r="A1" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21">
+    <row r="2" spans="1:18" ht="21">
       <c r="A2" s="3" t="s">
         <v>160</v>
       </c>
@@ -1260,7 +1374,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1271,25 +1385,37 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4" t="s">
         <v>199</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H4" t="s">
-        <v>200</v>
-      </c>
       <c r="I4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>201</v>
+      </c>
+      <c r="M4" t="s">
+        <v>222</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="O4" t="s">
+        <v>230</v>
+      </c>
+      <c r="P4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -1317,10 +1443,16 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N5" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1334,7 +1466,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1344,13 +1476,20 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>213</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N6" s="22">
+        <v>35</v>
+      </c>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1374,13 +1513,20 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>213</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N7" s="22">
+        <v>8</v>
+      </c>
+      <c r="O7" s="14"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1404,10 +1550,17 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N8" s="22">
+        <v>8</v>
+      </c>
+      <c r="O8" s="14"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1431,10 +1584,17 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N9" s="22">
+        <v>6</v>
+      </c>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1458,10 +1618,18 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="N10" s="26">
+        <v>4</v>
+      </c>
+      <c r="O10" s="25"/>
+      <c r="R10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1485,10 +1653,17 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N11" s="22">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1512,10 +1687,22 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N12" s="22">
+        <v>3</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1539,10 +1726,17 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N13" s="22">
+        <v>5</v>
+      </c>
+      <c r="O13" s="14"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1566,10 +1760,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1593,10 +1795,21 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>214</v>
+      </c>
+      <c r="M15" s="14"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="R15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1624,10 +1837,17 @@
         <v>6.9599999999999991</v>
       </c>
       <c r="J16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1655,10 +1875,16 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="J17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N17" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1686,10 +1912,17 @@
         <v>2.0640000000000001</v>
       </c>
       <c r="J18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N18" s="19"/>
+      <c r="O18" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1706,21 +1939,28 @@
         <v>170</v>
       </c>
       <c r="F19" s="6">
-        <v>2311129</v>
+        <v>3882627</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="7">
-        <v>0.46200000000000002</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="I19" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>4.1580000000000004</v>
+        <v>3.528</v>
       </c>
       <c r="J19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1748,10 +1988,16 @@
         <v>0.313</v>
       </c>
       <c r="J20" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1759,7 +2005,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D21" s="5">
         <v>3</v>
@@ -1779,13 +2025,21 @@
         <v>1.26</v>
       </c>
       <c r="J21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>213</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N21" s="22">
+        <v>7</v>
+      </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1793,7 +2047,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D22" s="5">
         <v>3</v>
@@ -1813,10 +2067,19 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="J22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N22" s="19">
+        <v>2</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P22" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1844,10 +2107,17 @@
         <v>2.29</v>
       </c>
       <c r="J23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N23" s="19"/>
+      <c r="O23" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1855,7 +2125,7 @@
         <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>232</v>
       </c>
       <c r="D24" s="5">
         <v>8</v>
@@ -1864,7 +2134,7 @@
         <v>168</v>
       </c>
       <c r="F24" s="6">
-        <v>1852699</v>
+        <v>2453214</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7">
@@ -1875,10 +2145,17 @@
         <v>2.88</v>
       </c>
       <c r="J24" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N24" s="19"/>
+      <c r="O24" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1906,10 +2183,17 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="J25" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N25" s="19"/>
+      <c r="O25" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1926,7 +2210,7 @@
         <v>167</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7"/>
@@ -1935,10 +2219,20 @@
         <v>0</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N26" s="19"/>
+      <c r="O26" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1966,13 +2260,19 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="J27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>216</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N27" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2000,25 +2300,33 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="J28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>216</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N28" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>45</v>
       </c>
       <c r="B29" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="D29" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="F29" s="6">
         <v>2217974</v>
@@ -2029,347 +2337,436 @@
       </c>
       <c r="I29" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>1.0379999999999998</v>
+        <v>0.51899999999999991</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N29" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D30" s="5">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" s="6">
+        <v>2290331</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="14"/>
+      <c r="M30" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="N30" s="19">
+        <v>1</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
+      <c r="R30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D31" s="5">
         <v>4</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F31" s="6">
         <v>1330733</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H30" s="7">
+      <c r="G31" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H31" s="7">
         <v>3.35</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I31" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
         <v>13.4</v>
       </c>
-      <c r="J30" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
+      <c r="J31" t="s">
+        <v>214</v>
+      </c>
+      <c r="M31" s="23"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="23"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
         <v>157</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7">
-        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7">
+        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N32" s="19">
         <v>4</v>
       </c>
-      <c r="F32" s="6">
-        <v>2393507</v>
-      </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7">
-        <v>1.92</v>
-      </c>
-      <c r="I32" s="7">
-        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>1.92</v>
-      </c>
-      <c r="J32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="F33" s="6">
-        <v>2393509</v>
+        <v>2393507</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="7">
-        <v>2.62</v>
+        <v>1.38</v>
       </c>
       <c r="I33" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>2.62</v>
+        <v>1.38</v>
       </c>
       <c r="J33" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N33" s="19"/>
+      <c r="O33" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="F34" s="6">
-        <v>2112375</v>
+        <v>2393509</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="7">
-        <v>1.55</v>
+        <v>1.83</v>
       </c>
       <c r="I34" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>1.55</v>
+        <v>1.83</v>
       </c>
       <c r="J34" t="s">
-        <v>215</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="N34" s="19"/>
+      <c r="O34" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F35" s="6">
-        <v>1098043</v>
+        <v>2112375</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="7">
-        <v>1.18</v>
+        <v>1.55</v>
       </c>
       <c r="I35" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>2.36</v>
+        <v>1.55</v>
       </c>
       <c r="J35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N35" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="D36" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="F36" s="6">
-        <v>9845330</v>
+        <v>1098043</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="7">
+        <v>1.18</v>
+      </c>
+      <c r="I36" s="7">
+        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
+        <v>2.36</v>
+      </c>
+      <c r="J36" t="s">
+        <v>214</v>
+      </c>
+      <c r="N36" s="19"/>
+      <c r="O36" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="6">
+        <v>9845330</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="7">
         <v>0.20599999999999999</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I37" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
         <v>0.61799999999999999</v>
       </c>
-      <c r="J36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" t="s">
+      <c r="J37" t="s">
+        <v>214</v>
+      </c>
+      <c r="N37" s="19">
+        <v>2</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D38" s="5">
         <v>2</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7">
+      <c r="F38" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
         <v>0</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" t="s">
-        <v>212</v>
-      </c>
-      <c r="B38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F38" s="6">
-        <v>2323482</v>
-      </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="7">
-        <v>21.38</v>
-      </c>
-      <c r="I38" s="7">
-        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>21.38</v>
-      </c>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="J38" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N38" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="B39" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="6">
+        <v>2323482</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7">
+        <v>21.38</v>
+      </c>
+      <c r="I39" s="7">
+        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
+        <v>21.38</v>
+      </c>
+      <c r="J39" s="16"/>
+      <c r="M39" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="R39" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="5">
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="5">
         <v>2</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H39" s="7">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H40" s="7">
         <v>18.510000000000002</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I40" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
         <v>37.020000000000003</v>
       </c>
-      <c r="J39" s="16"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="5">
-        <v>1</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7">
-        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="J40" s="16"/>
+      <c r="M40" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N40" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -2377,13 +2774,13 @@
         <v>65</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D41" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>163</v>
+        <v>62</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -2393,26 +2790,35 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N41" s="22">
+        <v>3</v>
+      </c>
+      <c r="O41" s="14"/>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="1">
-        <v>47</v>
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D42" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F42" s="6"/>
+        <v>163</v>
+      </c>
+      <c r="F42" s="6">
+        <v>2116438</v>
+      </c>
       <c r="G42" s="6"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7">
@@ -2420,10 +2826,20 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M42" s="14"/>
+      <c r="N42" s="22">
+        <v>2</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2431,13 +2847,13 @@
         <v>60</v>
       </c>
       <c r="C43" s="1">
-        <v>120</v>
+        <v>47</v>
       </c>
       <c r="D43" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2447,10 +2863,17 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N43" s="22">
+        <v>98</v>
+      </c>
+      <c r="O43" s="14"/>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2458,13 +2881,13 @@
         <v>60</v>
       </c>
       <c r="C44" s="1">
-        <v>270</v>
+        <v>120</v>
       </c>
       <c r="D44" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2474,10 +2897,15 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N44" s="22"/>
+      <c r="O44" s="14"/>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2485,13 +2913,13 @@
         <v>60</v>
       </c>
       <c r="C45" s="1">
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="D45" s="5">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2501,10 +2929,15 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M45" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N45" s="22"/>
+      <c r="O45" s="14"/>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2512,13 +2945,13 @@
         <v>60</v>
       </c>
       <c r="C46" s="1">
-        <v>470</v>
+        <v>330</v>
       </c>
       <c r="D46" s="5">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2528,10 +2961,17 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N46" s="22">
+        <v>70</v>
+      </c>
+      <c r="O46" s="14"/>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2539,13 +2979,13 @@
         <v>60</v>
       </c>
       <c r="C47" s="1">
-        <v>680</v>
+        <v>470</v>
       </c>
       <c r="D47" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2555,24 +2995,31 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+        <v>214</v>
+      </c>
+      <c r="M47" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N47" s="22">
+        <v>100</v>
+      </c>
+      <c r="O47" s="14"/>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" t="s">
         <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>75</v>
+      <c r="C48" s="1">
+        <v>680</v>
       </c>
       <c r="D48" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>191</v>
+        <v>74</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2582,10 +3029,17 @@
         <v>0</v>
       </c>
       <c r="J48" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M48" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N48" s="22">
+        <v>9</v>
+      </c>
+      <c r="O48" s="14"/>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2593,13 +3047,13 @@
         <v>60</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D49" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>70</v>
+        <v>191</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -2609,10 +3063,15 @@
         <v>0</v>
       </c>
       <c r="J49" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N49" s="22"/>
+      <c r="O49" s="14"/>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -2620,13 +3079,13 @@
         <v>60</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D50" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>195</v>
+        <v>70</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -2636,10 +3095,15 @@
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M50" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N50" s="22"/>
+      <c r="O50" s="14"/>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2647,13 +3111,13 @@
         <v>60</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D51" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -2663,10 +3127,17 @@
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M51" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N51" s="22">
+        <v>90</v>
+      </c>
+      <c r="O51" s="14"/>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2674,13 +3145,13 @@
         <v>60</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D52" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -2690,10 +3161,15 @@
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M52" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N52" s="22"/>
+      <c r="O52" s="14"/>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2701,13 +3177,13 @@
         <v>60</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>221</v>
+        <v>77</v>
       </c>
       <c r="D53" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -2717,10 +3193,15 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N53" s="22"/>
+      <c r="O53" s="14"/>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2728,13 +3209,13 @@
         <v>60</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>68</v>
+        <v>220</v>
       </c>
       <c r="D54" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -2744,10 +3225,15 @@
         <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N54" s="22"/>
+      <c r="O54" s="14"/>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2755,13 +3241,13 @@
         <v>60</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -2771,10 +3257,15 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M55" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N55" s="22"/>
+      <c r="O55" s="14"/>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -2782,13 +3273,13 @@
         <v>60</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>222</v>
+        <v>73</v>
       </c>
       <c r="D56" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -2798,87 +3289,105 @@
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M56" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N56" s="22"/>
+      <c r="O56" s="14"/>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="5">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7">
+        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>214</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N57" s="22">
+        <v>47</v>
+      </c>
+      <c r="O57" s="14"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
         <v>54</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D57" s="5">
-        <v>1</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F57" s="6">
-        <v>1141392</v>
-      </c>
-      <c r="G57" s="6"/>
-      <c r="H57" s="7">
-        <v>1.59</v>
-      </c>
-      <c r="I57" s="7">
-        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>1.59</v>
-      </c>
-      <c r="J57" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" t="s">
-        <v>139</v>
-      </c>
-      <c r="B58" t="s">
-        <v>140</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>203</v>
+        <v>53</v>
+      </c>
+      <c r="F58" s="6">
+        <v>1141392</v>
       </c>
       <c r="G58" s="6"/>
-      <c r="H58" s="7"/>
+      <c r="H58" s="7">
+        <v>1.59</v>
+      </c>
       <c r="I58" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>1.59</v>
+      </c>
+      <c r="J58" t="s">
+        <v>214</v>
+      </c>
+      <c r="M58" s="14"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B59" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="7"/>
@@ -2887,74 +3396,90 @@
         <v>0</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N59" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="6">
-        <v>2484971</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="H60" s="7">
-        <v>15.86</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="7"/>
       <c r="I60" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>15.86</v>
-      </c>
-      <c r="J60" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="J60" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N60" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F61" s="6">
-        <v>1672130</v>
-      </c>
-      <c r="G61" s="6"/>
+        <v>2484971</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>208</v>
+      </c>
       <c r="H61" s="7">
-        <v>5.5</v>
+        <v>15.86</v>
       </c>
       <c r="I61" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>5.5</v>
+        <v>15.86</v>
       </c>
       <c r="J61" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N61" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -2962,30 +3487,36 @@
         <v>124</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F62" s="6">
-        <v>1696319</v>
+        <v>1672130</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="7">
-        <v>7.1</v>
+        <v>5.5</v>
       </c>
       <c r="I62" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>7.1</v>
+        <v>5.5</v>
       </c>
       <c r="J62" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M62" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N62" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -2993,118 +3524,154 @@
         <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D63" s="5">
         <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F63" s="6">
-        <v>1696320</v>
+        <v>1696319</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="7">
-        <v>4.4000000000000004</v>
+        <v>7.1</v>
       </c>
       <c r="I63" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
-        <v>4.4000000000000004</v>
+        <v>7.1</v>
       </c>
       <c r="J63" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="M63" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N63" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="D64" s="5">
         <v>1</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="F64" s="6">
-        <v>2308726</v>
+        <v>1696320</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I64" s="7">
+        <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J64" t="s">
+        <v>214</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N64" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="6">
+        <v>2308726</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="H65" s="7">
         <v>1.43</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I65" s="7">
         <f>Table2[[#This Row],[Qty]]*Table2[[#This Row],[P.U.]]</f>
         <v>1.43</v>
       </c>
-      <c r="J64" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="H65" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="I65" s="11">
+      <c r="J65" t="s">
+        <v>214</v>
+      </c>
+      <c r="N65" s="19"/>
+      <c r="O65" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="H66" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I66" s="11">
         <f>SUM(Table2[Total])</f>
-        <v>141.06299999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="H66" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I66" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>138.58400000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="H67" s="10" t="s">
         <v>205</v>
       </c>
       <c r="I67" s="11">
-        <f>(I65+I66)*0.2</f>
-        <v>30.6126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="H68" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="I68" s="9">
-        <f>I65+I67</f>
-        <v>171.67559999999997</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="15"/>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174" t="s">
-        <v>78</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C174" t="s">
-        <v>59</v>
-      </c>
-      <c r="D174" t="s">
-        <v>60</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="H68" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="I68" s="11">
+        <f>(I66+I67)*0.2</f>
+        <v>30.116800000000008</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="H69" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="I69" s="9">
+        <f>I66+I68</f>
+        <v>168.70080000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" s="15"/>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>79</v>
-      </c>
-      <c r="B175" s="1">
-        <v>330</v>
+        <v>78</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C175" t="s">
         <v>59</v>
@@ -3115,10 +3682,10 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>80</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="B176" s="1">
+        <v>330</v>
       </c>
       <c r="C176" t="s">
         <v>59</v>
@@ -3129,10 +3696,10 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>81</v>
-      </c>
-      <c r="B177" s="1">
-        <v>330</v>
+        <v>80</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C177" t="s">
         <v>59</v>
@@ -3143,10 +3710,10 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>82</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="B178" s="1">
+        <v>330</v>
       </c>
       <c r="C178" t="s">
         <v>59</v>
@@ -3157,10 +3724,10 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>83</v>
-      </c>
-      <c r="B179" s="1">
-        <v>330</v>
+        <v>82</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C179" t="s">
         <v>59</v>
@@ -3171,10 +3738,10 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>84</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="B180" s="1">
+        <v>330</v>
       </c>
       <c r="C180" t="s">
         <v>59</v>
@@ -3185,10 +3752,10 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>85</v>
-      </c>
-      <c r="B181" s="1">
-        <v>330</v>
+        <v>84</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C181" t="s">
         <v>59</v>
@@ -3199,10 +3766,10 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>86</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="B182" s="1">
+        <v>330</v>
       </c>
       <c r="C182" t="s">
         <v>59</v>
@@ -3213,10 +3780,10 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>87</v>
-      </c>
-      <c r="B183" s="1">
-        <v>330</v>
+        <v>86</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C183" t="s">
         <v>59</v>
@@ -3227,10 +3794,10 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>88</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="B184" s="1">
+        <v>330</v>
       </c>
       <c r="C184" t="s">
         <v>59</v>
@@ -3241,10 +3808,10 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>89</v>
-      </c>
-      <c r="B185" s="1">
-        <v>330</v>
+        <v>88</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C185" t="s">
         <v>59</v>
@@ -3255,10 +3822,10 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>90</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
+      </c>
+      <c r="B186" s="1">
+        <v>330</v>
       </c>
       <c r="C186" t="s">
         <v>59</v>
@@ -3269,7 +3836,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>76</v>
@@ -3283,7 +3850,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>76</v>
@@ -3297,7 +3864,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>76</v>
@@ -3311,10 +3878,10 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C190" t="s">
         <v>59</v>
@@ -3325,10 +3892,10 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>95</v>
-      </c>
-      <c r="B191" s="1">
-        <v>330</v>
+        <v>94</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C191" t="s">
         <v>59</v>
@@ -3339,10 +3906,10 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>96</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="B192" s="1">
+        <v>330</v>
       </c>
       <c r="C192" t="s">
         <v>59</v>
@@ -3353,10 +3920,10 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>97</v>
-      </c>
-      <c r="B193" s="1">
-        <v>330</v>
+        <v>96</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C193" t="s">
         <v>59</v>
@@ -3367,10 +3934,10 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>98</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="B194" s="1">
+        <v>330</v>
       </c>
       <c r="C194" t="s">
         <v>59</v>
@@ -3381,10 +3948,10 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>99</v>
-      </c>
-      <c r="B195" s="1">
-        <v>330</v>
+        <v>98</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C195" t="s">
         <v>59</v>
@@ -3395,10 +3962,10 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>100</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
+      </c>
+      <c r="B196" s="1">
+        <v>330</v>
       </c>
       <c r="C196" t="s">
         <v>59</v>
@@ -3409,10 +3976,10 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>101</v>
-      </c>
-      <c r="B197" s="1">
-        <v>330</v>
+        <v>100</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C197" t="s">
         <v>59</v>
@@ -3423,10 +3990,10 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B198" s="1">
-        <v>120</v>
+        <v>330</v>
       </c>
       <c r="C198" t="s">
         <v>59</v>
@@ -3437,7 +4004,7 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B199" s="1">
         <v>120</v>
@@ -3451,10 +4018,10 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>104</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>76</v>
+        <v>103</v>
+      </c>
+      <c r="B200" s="1">
+        <v>120</v>
       </c>
       <c r="C200" t="s">
         <v>59</v>
@@ -3465,10 +4032,10 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>105</v>
-      </c>
-      <c r="B201" s="1">
-        <v>120</v>
+        <v>104</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C201" t="s">
         <v>59</v>
@@ -3479,88 +4046,88 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>106</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="B202" s="1">
+        <v>120</v>
       </c>
       <c r="C202" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="D202" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C203" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D203" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>112</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C204" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D204" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C205" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D205" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>118</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C206" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D206" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C207" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D207" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C208" t="s">
         <v>123</v>
@@ -3571,10 +4138,10 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C209" t="s">
         <v>123</v>
@@ -3585,88 +4152,88 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C210" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D210" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>132</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C211" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D211" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C212" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D212" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C213" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D213" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C214" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D214" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C215" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D215" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>145</v>
@@ -3680,10 +4247,10 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C217" t="s">
         <v>145</v>
@@ -3694,21 +4261,21 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="C218" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="D218" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>47</v>
@@ -3722,7 +4289,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>47</v>
@@ -3736,7 +4303,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>47</v>
@@ -3750,7 +4317,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>47</v>
@@ -3764,7 +4331,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>47</v>
@@ -3778,19 +4345,36 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
+        <v>155</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C224" t="s">
+        <v>47</v>
+      </c>
+      <c r="D224" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" t="s">
         <v>156</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B225" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C225" t="s">
         <v>158</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D225" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M39:O39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>